<commit_message>
add new param n for guessing col_type
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomask/Documents/Soziologie/R/R-Packages/forked pkges/readxl/tests/testthat/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24800" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,12 +45,18 @@
     <t>ab</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>string_at_102</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -80,10 +91,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -406,17 +422,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +445,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -444,9 +463,8 @@
         <v>38717</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
-        <f>1+0</f>
         <v>1</v>
       </c>
       <c r="B3" t="str">
@@ -462,14 +480,506 @@
         <v>38717</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add guess_max param for guessing col_type; fixes #223 (#257)
* add new param n for guessing col_type

* Rename `n` to `guess_max`

* Account for explicit skip in xls col type processing

* Tests re: col types and the new guess_max parameter

* Use guess_max checking and tests from readr

* guess_max EVERYWHERE and consistent default to 1000

* Add NEWS bullet re: guess_max

* oops
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,13 +47,19 @@
   <si>
     <t>ab</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>string_in_row_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -83,7 +97,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -406,17 +425,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +448,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,33 +465,39 @@
       <c r="D2" s="1">
         <v>38717</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
-        <f>1+0</f>
         <v>1</v>
       </c>
-      <c r="B3" t="str">
-        <f>CONCATENATE("a", "b")</f>
-        <v>ab</v>
-      </c>
       <c r="C3" t="b">
-        <f>"a"="b"</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <f>D2</f>
         <v>38717</v>
       </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <f>CONCATENATE("a", "b")</f>
+        <v>ab</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle xls record type BoolErr (number 517); fixes #259, relates to #270, relates to #62
This record type is also used for errors, but only errors that are not a result of a formula, which is most of them. So if OP on #62 provides an example, we could conceivably do more in the else branch here.
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="7820" yWindow="460" windowWidth="20980" windowHeight="8600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>string_in_row_3</t>
+  </si>
+  <si>
+    <t>errors</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,13 +449,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,31 +466,38 @@
         <v>4</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E2" s="1">
         <v>38717</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <f>D2</f>
+        <v>0</v>
+      </c>
+      <c r="D3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="1">
+        <f>E2</f>
         <v>38717</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -492,7 +505,11 @@
         <f>CONCATENATE("a", "b")</f>
         <v>ab</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="e">
+        <f>F2+F4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handle xls record type BoolErr (number 517); fixes #259, relates to #… (#274)
* Handle xls record type BoolErr (number 517); fixes #259, relates to #270, relates to #62

This record type is also used for errors, but only errors that are not a result of a formula, which is most of them. So if OP on #62 provides an example, we could conceivably do more in the else branch here.

* Fix NEWS
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="7820" yWindow="460" windowWidth="20980" windowHeight="8600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>string_in_row_3</t>
+  </si>
+  <si>
+    <t>errors</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,13 +449,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,31 +466,38 @@
         <v>4</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E2" s="1">
         <v>38717</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <f>D2</f>
+        <v>0</v>
+      </c>
+      <c r="D3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="1">
+        <f>E2</f>
         <v>38717</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -492,7 +505,11 @@
         <f>CONCATENATE("a", "b")</f>
         <v>ab</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="e">
+        <f>F2+F4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add logical cell and col types; general refactor of cell typing and coercion
Rescues xls formula dates
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,10 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="460" windowWidth="20980" windowHeight="8600" tabRatio="500"/>
+    <workbookView xWindow="6720" yWindow="920" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="guess_me" sheetId="2" r:id="rId1"/>
+    <sheet name="guess_max" sheetId="1" r:id="rId2"/>
+    <sheet name="smorgasbord" sheetId="3" r:id="rId3"/>
+    <sheet name="logical_coercion" sheetId="4" r:id="rId4"/>
+    <sheet name="date_coercion" sheetId="5" r:id="rId5"/>
+    <sheet name="numeric_coercion" sheetId="6" r:id="rId6"/>
+    <sheet name="text_coercion" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,41 +33,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>string_in_row_3</t>
+  </si>
+  <si>
+    <t>blank</t>
   </si>
   <si>
     <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>string_in_row_3</t>
-  </si>
-  <si>
-    <t>errors</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>hello world</t>
+  </si>
+  <si>
+    <t>text formula</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>numeric formula</t>
+  </si>
+  <si>
+    <t>boolean true</t>
+  </si>
+  <si>
+    <t>boolean false</t>
+  </si>
+  <si>
+    <t>boolean formula true</t>
+  </si>
+  <si>
+    <t>boolean formula false</t>
+  </si>
+  <si>
+    <t>date formula</t>
+  </si>
+  <si>
+    <t>error #N/A explicit</t>
+  </si>
+  <si>
+    <t>error #N/A formula</t>
+  </si>
+  <si>
+    <t>error #NAME?</t>
+  </si>
+  <si>
+    <t>error #VALUE!</t>
+  </si>
+  <si>
+    <t>error #DIV/0!</t>
+  </si>
+  <si>
+    <t>error #REF</t>
+  </si>
+  <si>
+    <t>error #NUM!</t>
+  </si>
+  <si>
+    <t>error  #NULL!</t>
+  </si>
+  <si>
+    <t>cabbage</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>foo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -92,9 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,92 +503,539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41331</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>41332</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D2+1</f>
+        <v>41332</v>
+      </c>
+      <c r="E5">
+        <f>E2+E3</f>
+        <v>3</v>
+      </c>
+      <c r="F5" t="str">
+        <f>UPPER(F2)</f>
+        <v>HELLO</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C6" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>D3-1</f>
+        <v>41331</v>
+      </c>
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
+        <v>6</v>
+      </c>
+      <c r="F6" t="str">
+        <f>LEFT(F3,3)</f>
+        <v>wor</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="e">
-        <f>1/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="1">
-        <v>38717</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="1">
-        <f>E2</f>
-        <v>38717</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <f>CONCATENATE("a", "b")</f>
-        <v>ab</v>
-      </c>
-      <c r="D4" t="e">
-        <f>F2+F4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="str">
+        <f>UPPER(B1)</f>
+        <v>HELLO WORLD</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>B4^2</f>
+        <v>1.6900000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B11+5</f>
+        <v>40969</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="e">
+        <f ca="1">su(B4)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="e">
+        <f>B4+B1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="e">
+        <f>SQRT(-2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="e">
+        <f>SUM(A2 A6)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>"F"</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>40908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>41051</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>39529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>39335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>40534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>41175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Attempt to coerce text to number; fixes #217, fixes #106
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="920" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="8620" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>ab</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>foo</t>
+  </si>
+  <si>
+    <t>72</t>
   </si>
 </sst>
 </file>
@@ -153,9 +156,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -165,10 +177,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +521,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -830,7 +845,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -938,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -958,8 +973,8 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>-2</v>
+      <c r="A3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
@@ -991,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Coerce numeric to date in a "date" column; fixes #266
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -177,13 +177,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,11 +904,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -935,8 +939,8 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>39529</v>
+      <c r="A7" s="4">
+        <v>39448</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
@@ -953,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Beef up tests of logical coercion; delete old coercion test that adds nothing
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>ab</t>
   </si>
@@ -129,6 +129,36 @@
   </si>
   <si>
     <t>72</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>static logical</t>
+  </si>
+  <si>
+    <t>formula logical</t>
+  </si>
+  <si>
+    <t>string logical</t>
+  </si>
+  <si>
+    <t>string not logical</t>
   </si>
 </sst>
 </file>
@@ -177,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -185,6 +215,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +656,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection sqref="A1:E65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -843,10 +874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -854,45 +885,149 @@
     <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" t="str">
-        <f>"F"</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>"false"</f>
+        <v>false</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>40908</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" t="b">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add logical cell & col types; refactor cell typing and coercion (#277)
* Add logical cell and col types; general refactor of cell typing and coercion

Rescues xls formula dates

* Make logicalFromString() to use in xls and xlsx

* Attempt to coerce text to number; fixes #217, fixes #106

* Work on NEWS.md

* Fiddle with comments and kick appveyor

* Edit Xls[x]WorkSheet.h side-by-side for parallelism

* Edit NEWS.md

* Coerce numeric to date in a "date" column; fixes #266

* Don't use C++11 when converting string to double

* Test all the warnings

* Enhance comments and refactor xls cell typing

* Consistently use strncmp(this, that, n) == 0

* Simplify logical cell creation in xls

* Fewer parens

* Add comment, collapse two cases

* Use Rf_StringTrue() and Rf_StringFalse()

* Beef up tests of logical coercion; delete old coercion test that adds nothing

* Frontload comments re: xls & xlsx cell types and make more parallel
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="460" windowWidth="20980" windowHeight="8600" tabRatio="500"/>
+    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="guess_me" sheetId="2" r:id="rId1"/>
+    <sheet name="guess_max" sheetId="1" r:id="rId2"/>
+    <sheet name="smorgasbord" sheetId="3" r:id="rId3"/>
+    <sheet name="logical_coercion" sheetId="4" r:id="rId4"/>
+    <sheet name="date_coercion" sheetId="5" r:id="rId5"/>
+    <sheet name="numeric_coercion" sheetId="6" r:id="rId6"/>
+    <sheet name="text_coercion" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,41 +33,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>string_in_row_3</t>
+  </si>
+  <si>
+    <t>blank</t>
   </si>
   <si>
     <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>string_in_row_3</t>
-  </si>
-  <si>
-    <t>errors</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>hello world</t>
+  </si>
+  <si>
+    <t>text formula</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>numeric formula</t>
+  </si>
+  <si>
+    <t>boolean true</t>
+  </si>
+  <si>
+    <t>boolean false</t>
+  </si>
+  <si>
+    <t>boolean formula true</t>
+  </si>
+  <si>
+    <t>boolean formula false</t>
+  </si>
+  <si>
+    <t>date formula</t>
+  </si>
+  <si>
+    <t>error #N/A explicit</t>
+  </si>
+  <si>
+    <t>error #N/A formula</t>
+  </si>
+  <si>
+    <t>error #NAME?</t>
+  </si>
+  <si>
+    <t>error #VALUE!</t>
+  </si>
+  <si>
+    <t>error #DIV/0!</t>
+  </si>
+  <si>
+    <t>error #REF</t>
+  </si>
+  <si>
+    <t>error #NUM!</t>
+  </si>
+  <si>
+    <t>error  #NULL!</t>
+  </si>
+  <si>
+    <t>cabbage</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>static logical</t>
+  </si>
+  <si>
+    <t>formula logical</t>
+  </si>
+  <si>
+    <t>string logical</t>
+  </si>
+  <si>
+    <t>string not logical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -80,9 +186,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -92,9 +207,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,92 +550,646 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41331</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>41332</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D2+1</f>
+        <v>41332</v>
+      </c>
+      <c r="E5">
+        <f>E2+E3</f>
+        <v>3</v>
+      </c>
+      <c r="F5" t="str">
+        <f>UPPER(F2)</f>
+        <v>HELLO</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="C6" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>D3-1</f>
+        <v>41331</v>
+      </c>
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
+        <v>6</v>
+      </c>
+      <c r="F6" t="str">
+        <f>LEFT(F3,3)</f>
+        <v>wor</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="e">
-        <f>1/0</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" s="1">
-        <v>38717</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="1">
-        <f>E2</f>
-        <v>38717</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="str">
-        <f>CONCATENATE("a", "b")</f>
-        <v>ab</v>
-      </c>
-      <c r="D4" t="e">
-        <f>F2+F4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="str">
+        <f>UPPER(B1)</f>
+        <v>HELLO WORLD</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>B4^2</f>
+        <v>1.6900000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B11+5</f>
+        <v>40969</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="e">
+        <f ca="1">su(B4)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="e">
+        <f>B4+B1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="e">
+        <f>SQRT(-2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="e">
+        <f>SUM(A2 A6)</f>
+        <v>#NULL!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>"false"</f>
+        <v>false</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>40908</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>41051</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>39335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>40534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>41175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tests inspired by fact this closes #75, closes #110
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2880" yWindow="1160" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>ab</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>string not logical</t>
+  </si>
+  <si>
+    <t>logical F</t>
+  </si>
+  <si>
+    <t>floating point</t>
   </si>
 </sst>
 </file>
@@ -876,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1143,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1154,39 +1160,65 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>41175</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Align cell methods between xls and xlsx (#287)
* xlsx: Use cell type information when extracting/coercing contents

* xls: add asStdString() and asCharSxp()

* xls: add asInteger()

* xls: add asDouble()

* xls: add asDate()

* xls: all readCols() cell access must be via an asWhatever() method

* xls: don't export direct accessor of the xls cell

* xls: all colNames() cell access must be via an asWhatever() method

* Grooming for parallelism

* Tests inspired by fact this closes #75, closes #110
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="1140" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2880" yWindow="1160" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>ab</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>string not logical</t>
+  </si>
+  <si>
+    <t>logical F</t>
+  </si>
+  <si>
+    <t>floating point</t>
   </si>
 </sst>
 </file>
@@ -876,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1143,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1154,39 +1160,65 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>41175</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve coercion of numbers to text in xls; fixes #298
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>ab</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>floating point</t>
+  </si>
+  <si>
+    <t>student number</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1221,6 +1224,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>36436153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve coercion of numbers to text in xls; fixes #298 (#305)
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>ab</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>floating point</t>
+  </si>
+  <si>
+    <t>student number</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1221,6 +1224,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>36436153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
"it works for xls"
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/types.xlsx
+++ b/tests/testthat/sheets/types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1160" windowWidth="20980" windowHeight="13980" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2880" yWindow="1160" windowWidth="20980" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="guess_me" sheetId="2" r:id="rId1"/>
@@ -559,98 +559,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>41331</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41332</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C2+1</f>
+        <v>41332</v>
+      </c>
+      <c r="D5">
+        <f>D2+D3</f>
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>41331</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>41332</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <f>D2+1</f>
-        <v>41332</v>
-      </c>
-      <c r="E5">
-        <f>E2+E3</f>
-        <v>3</v>
-      </c>
-      <c r="F5" t="str">
-        <f>UPPER(F2)</f>
+      <c r="E5" t="str">
+        <f>UPPER(E2)</f>
         <v>HELLO</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C6" t="b">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D6" s="1">
-        <f>D3-1</f>
+      <c r="C6" s="1">
+        <f>C3-1</f>
         <v>41331</v>
       </c>
-      <c r="E6">
-        <f>SUM(E2:E5)</f>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
         <v>6</v>
       </c>
-      <c r="F6" t="str">
-        <f>LEFT(F3,3)</f>
+      <c r="E6" t="str">
+        <f>LEFT(E3,3)</f>
         <v>wor</v>
       </c>
     </row>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>